<commit_message>
Finished adding items to the BOM, added a tactile switch from JLCPCB footprint instead of the one I had
</commit_message>
<xml_diff>
--- a/bom_manual.xlsx
+++ b/bom_manual.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\Documents\KiCad\Rocketboard-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6C7E57-D9C7-4A3C-9E4B-5A5916BFE95B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330DA346-2FE1-41CC-9E70-3A689C8F1D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38265" yWindow="2895" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="157">
   <si>
     <t>Qty</t>
   </si>
@@ -390,9 +398,6 @@
     <t>Cannot find anywhere but AliExpress, will have to be hand soldered for the time being</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Nothing to be loaded</t>
   </si>
   <si>
@@ -433,6 +438,72 @@
   </si>
   <si>
     <t>Not carried by JLCPCB - mounting pins may not be long enough for 1.6mm board!</t>
+  </si>
+  <si>
+    <t>0603WAF200JT5E</t>
+  </si>
+  <si>
+    <t>C22950</t>
+  </si>
+  <si>
+    <t>Uniroyal Elec</t>
+  </si>
+  <si>
+    <t>0603WAF1002T5E</t>
+  </si>
+  <si>
+    <t>C25804</t>
+  </si>
+  <si>
+    <t>0603WAF5101T5E</t>
+  </si>
+  <si>
+    <t>C23186</t>
+  </si>
+  <si>
+    <t>0603WAF1501T5E</t>
+  </si>
+  <si>
+    <t>C22843</t>
+  </si>
+  <si>
+    <t>0603WAF1001T5E</t>
+  </si>
+  <si>
+    <t>C21190</t>
+  </si>
+  <si>
+    <t>TS-1187A-C-C-B</t>
+  </si>
+  <si>
+    <t>C318889</t>
+  </si>
+  <si>
+    <t>XKB Enterprise</t>
+  </si>
+  <si>
+    <t>EC11E1534408</t>
+  </si>
+  <si>
+    <t>C278348</t>
+  </si>
+  <si>
+    <t>ALPS Electric</t>
+  </si>
+  <si>
+    <t>C8734</t>
+  </si>
+  <si>
+    <t>Total Cost:</t>
+  </si>
+  <si>
+    <t>Board Cost</t>
+  </si>
+  <si>
+    <t>JLCPCB Cost:</t>
+  </si>
+  <si>
+    <t>Other Cost:</t>
   </si>
 </sst>
 </file>
@@ -499,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -513,6 +584,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -794,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,13 +883,13 @@
     <col min="5" max="5" width="17.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="24.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="80.109375" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="80.109375" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -846,11 +920,14 @@
       <c r="J1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -875,11 +952,19 @@
       <c r="H2" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="I2" s="1" t="str">
+        <f>IF(F2="JLCPCB ", "", "Yes")</f>
+        <v/>
+      </c>
       <c r="J2" s="5">
         <v>8.5000000000000006E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2" s="5">
+        <f>J2*A2</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -904,14 +989,22 @@
       <c r="H3" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I30" si="0">IF(F3="JLCPCB ", "", "Yes")</f>
+        <v/>
+      </c>
       <c r="J3" s="5">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:K30" si="1">J3*A3</f>
+        <v>1.66E-2</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>23</v>
       </c>
@@ -936,11 +1029,19 @@
       <c r="H4" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J4" s="5">
         <v>6.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K4" s="5">
+        <f t="shared" si="1"/>
+        <v>0.15639999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -965,14 +1066,22 @@
       <c r="H5" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J5" s="5">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="5">
+        <f t="shared" si="1"/>
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -997,14 +1106,22 @@
       <c r="H6" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J6" s="5">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1029,11 +1146,19 @@
       <c r="H7" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J7" s="5">
         <v>0.15490000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.15490000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1058,11 +1183,19 @@
       <c r="H8" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J8" s="5">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="5">
+        <f t="shared" si="1"/>
+        <v>1.29E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>19</v>
       </c>
@@ -1087,11 +1220,19 @@
       <c r="H9" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J9" s="5">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>16</v>
       </c>
@@ -1113,17 +1254,22 @@
       <c r="H10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>121</v>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
       </c>
       <c r="J10" s="5">
         <v>0.10489999999999999</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="5">
+        <f t="shared" si="1"/>
+        <v>1.6783999999999999</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1136,14 +1282,19 @@
       <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1156,14 +1307,19 @@
       <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1176,14 +1332,19 @@
       <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1196,14 +1357,19 @@
       <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>16</v>
       </c>
@@ -1216,14 +1382,19 @@
       <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1237,28 +1408,33 @@
         <v>42</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>121</v>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
       </c>
       <c r="J16" s="5">
         <v>0.84499999999999997</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K16" s="5">
+        <f t="shared" si="1"/>
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -1271,8 +1447,31 @@
       <c r="D17" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J17" s="5">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>3</v>
       </c>
@@ -1285,8 +1484,31 @@
       <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J18" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1299,8 +1521,31 @@
       <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J19" s="5">
+        <v>1.9E-3</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="1"/>
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1313,8 +1558,31 @@
       <c r="D20" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J20" s="5">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1327,8 +1595,31 @@
       <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J21" s="5">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="1"/>
+        <v>2.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1341,8 +1632,31 @@
       <c r="D22" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J22" s="5">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="1"/>
+        <v>3.4799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1355,8 +1669,31 @@
       <c r="D23" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1.943333</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="1"/>
+        <v>1.943333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1369,8 +1706,31 @@
       <c r="D24" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1.943333</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="1"/>
+        <v>1.943333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1383,8 +1743,31 @@
       <c r="D25" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J25" s="5">
+        <v>1.4413</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4413</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1409,11 +1792,19 @@
       <c r="H26" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J26" s="5">
         <v>0.124</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K26" s="5">
+        <f t="shared" si="1"/>
+        <v>0.124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1433,16 +1824,24 @@
         <v>78</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>127</v>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="J27" s="5">
         <v>9.1499999999999998E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="5">
+        <f t="shared" si="1"/>
+        <v>9.1499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -1456,22 +1855,30 @@
         <v>31</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="H28" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>131</v>
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
       </c>
       <c r="J28" s="5">
         <v>5.4961000000000003E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K28" s="5">
+        <f t="shared" si="1"/>
+        <v>5.4961000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1496,11 +1903,19 @@
       <c r="H29" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J29" s="5">
         <v>0.21870000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K29" s="5">
+        <f t="shared" si="1"/>
+        <v>0.21870000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -1525,11 +1940,53 @@
       <c r="H30" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J30" s="5">
         <v>0.2336</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="K30" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2336</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K33" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K34" s="5">
+        <f>SUMIF(I2:I30,"",K2:K30)</f>
+        <v>2.8732000000000002</v>
+      </c>
+      <c r="L34" s="7"/>
+    </row>
+    <row r="36" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K36" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K37" s="5">
+        <f>SUMIF(I2:I30, "yes", K2:K30)</f>
+        <v>6.4650269999999992</v>
+      </c>
+    </row>
+    <row r="39" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K39" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K40" s="5">
+        <f>K34+K37</f>
+        <v>9.3382269999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the graphics, added some more, and made some slight changed to some components
</commit_message>
<xml_diff>
--- a/bom_manual.xlsx
+++ b/bom_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seth\Documents\KiCad\Rocketboard-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330DA346-2FE1-41CC-9E70-3A689C8F1D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591D724D-EB74-4739-A29F-FDB5C4191FAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38265" yWindow="2895" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="160">
   <si>
     <t>Qty</t>
   </si>
@@ -504,6 +504,15 @@
   </si>
   <si>
     <t>Other Cost:</t>
+  </si>
+  <si>
+    <t>Unique parts (loaded) count:</t>
+  </si>
+  <si>
+    <t>Number of parts:</t>
+  </si>
+  <si>
+    <t>Number of loaded SMD parts:</t>
   </si>
 </sst>
 </file>
@@ -512,7 +521,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -580,11 +589,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -870,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1955,35 +1964,56 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H33" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="K33" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H34" s="1">
+        <f>COUNTBLANK(I2:I30)</f>
+        <v>19</v>
+      </c>
       <c r="K34" s="5">
         <f>SUMIF(I2:I30,"",K2:K30)</f>
         <v>2.8732000000000002</v>
       </c>
       <c r="L34" s="7"/>
     </row>
-    <row r="36" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H36" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="K36" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H37" s="1">
+        <f>SUMIF(I2:I30, "", A2:A30)</f>
+        <v>65</v>
+      </c>
       <c r="K37" s="5">
         <f>SUMIF(I2:I30, "yes", K2:K30)</f>
         <v>6.4650269999999992</v>
       </c>
     </row>
-    <row r="39" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H39" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="K39" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H40" s="1">
+        <f>SUM(A2:A30)</f>
+        <v>108</v>
+      </c>
       <c r="K40" s="5">
         <f>K34+K37</f>
         <v>9.3382269999999998</v>

</xml_diff>